<commit_message>
Consent.Status fixé à Active
Consent.Status fixé à Active caff832050c8c2e4080959accbd664a1a944b00f
</commit_message>
<xml_diff>
--- a/278-rc---esmsconsent---missing-status-constraint/ig/StructureDefinition-esms-consent.xlsx
+++ b/278-rc---esmsconsent---missing-status-constraint/ig/StructureDefinition-esms-consent.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-04T13:13:08+00:00</t>
+    <t>2024-12-04T13:27:24+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -4121,7 +4121,7 @@
         <v>76</v>
       </c>
       <c r="S20" t="s" s="2">
-        <v>76</v>
+        <v>10</v>
       </c>
       <c r="T20" t="s" s="2">
         <v>76</v>

</xml_diff>